<commit_message>
improve Wifi password management
</commit_message>
<xml_diff>
--- a/doc/PLsi.xlsx
+++ b/doc/PLsi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="642">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -108,7 +108,16 @@
     <t xml:space="preserve">Video / User Manual</t>
   </si>
   <si>
+    <t xml:space="preserve">screen with task monitoring watchdogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log file in chip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Build 2 units (1 analog 1 digital)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screen to confirm plc RUN or STOP</t>
   </si>
   <si>
     <t xml:space="preserve">Build 8 units</t>
@@ -3042,8 +3051,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3213,17 +3222,29 @@
       <c r="B13" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="E13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="E14" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,7 +3252,7 @@
         <v>0.5</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3247,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3271,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,7 +3308,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3311,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3327,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3353,17 +3374,17 @@
         <v>2</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3411,61 +3432,61 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="6"/>
@@ -3477,7 +3498,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="6"/>
@@ -3489,7 +3510,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
@@ -3501,7 +3522,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
@@ -3513,7 +3534,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
@@ -3549,7 +3570,7 @@
   </sheetPr>
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -3563,59 +3584,59 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3623,32 +3644,32 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E14" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E15" s="12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3657,120 +3678,120 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,7 +3799,7 @@
         <v>10</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,7 +3807,7 @@
         <v>100</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3794,7 +3815,7 @@
         <v>1000</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,7 +3823,7 @@
         <v>60000</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3813,50 +3834,50 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,103 +3886,103 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,98 +3991,98 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F74" s="10"/>
       <c r="G74" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4106,26 +4127,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G1" s="19"/>
       <c r="I1" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J1" s="20"/>
     </row>
@@ -4134,18 +4155,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G2" s="21"/>
       <c r="I2" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="J2" s="20"/>
       <c r="L2" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4153,26 +4174,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G3" s="21"/>
       <c r="I3" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,19 +4201,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G4" s="24"/>
       <c r="J4" s="20"/>
@@ -4202,30 +4223,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G5" s="21"/>
       <c r="I5" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4233,30 +4254,30 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G6" s="21"/>
       <c r="I6" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,32 +4285,32 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G7" s="21"/>
       <c r="I7" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4297,32 +4318,32 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G8" s="21"/>
       <c r="I8" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,32 +4351,32 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G9" s="21"/>
       <c r="I9" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4363,30 +4384,30 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G10" s="21"/>
       <c r="I10" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,30 +4415,30 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G11" s="21"/>
       <c r="I11" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,30 +4446,30 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G12" s="21"/>
       <c r="I12" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,30 +4477,30 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G13" s="21"/>
       <c r="I13" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4487,30 +4508,30 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G14" s="21"/>
       <c r="I14" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,30 +4539,30 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G15" s="21"/>
       <c r="I15" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4549,30 +4570,30 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G16" s="21"/>
       <c r="I16" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,30 +4601,30 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G17" s="21"/>
       <c r="I17" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4611,30 +4632,30 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>206</v>
-      </c>
       <c r="F18" s="23" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G18" s="25"/>
       <c r="I18" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4642,30 +4663,30 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G19" s="25"/>
       <c r="I19" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4673,30 +4694,30 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G20" s="25"/>
       <c r="I20" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4704,19 +4725,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G21" s="25"/>
     </row>
@@ -4725,23 +4746,23 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G22" s="25"/>
       <c r="I22" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4749,23 +4770,23 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G23" s="21"/>
       <c r="I23" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4773,26 +4794,26 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G24" s="21"/>
       <c r="I24" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,19 +4821,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G25" s="21"/>
       <c r="J25" s="0"/>
@@ -4822,19 +4843,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G26" s="21"/>
       <c r="J26" s="0"/>
@@ -4844,26 +4865,26 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G27" s="21"/>
       <c r="I27" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4871,23 +4892,23 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G28" s="21"/>
       <c r="J28" s="20" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4895,19 +4916,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G29" s="21"/>
       <c r="J29" s="20"/>
@@ -4917,23 +4938,23 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G30" s="21"/>
       <c r="I30" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4956,16 +4977,16 @@
       <c r="E32" s="0"/>
       <c r="G32" s="21"/>
       <c r="I32" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4978,16 +4999,16 @@
       <c r="E33" s="0"/>
       <c r="G33" s="21"/>
       <c r="I33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="L33" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5000,16 +5021,16 @@
       <c r="E34" s="0"/>
       <c r="G34" s="21"/>
       <c r="I34" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5022,16 +5043,16 @@
       <c r="E35" s="0"/>
       <c r="G35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5044,16 +5065,16 @@
       <c r="E36" s="0"/>
       <c r="G36" s="21"/>
       <c r="I36" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,16 +5107,16 @@
       <c r="E39" s="0"/>
       <c r="G39" s="21"/>
       <c r="I39" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,16 +5129,16 @@
       <c r="E40" s="0"/>
       <c r="G40" s="21"/>
       <c r="I40" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M40" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,16 +5151,16 @@
       <c r="E41" s="0"/>
       <c r="G41" s="21"/>
       <c r="I41" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M41" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,16 +5173,16 @@
       <c r="E42" s="0"/>
       <c r="G42" s="21"/>
       <c r="I42" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,16 +5195,16 @@
       <c r="E43" s="0"/>
       <c r="G43" s="21"/>
       <c r="I43" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M43" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5196,16 +5217,16 @@
       <c r="E44" s="0"/>
       <c r="G44" s="21"/>
       <c r="I44" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6618,13 +6639,13 @@
         <v>1001</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F303" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6632,13 +6653,13 @@
         <v>1002</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F304" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6646,13 +6667,13 @@
         <v>1003</v>
       </c>
       <c r="B305" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C305" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C305" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="F305" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6660,13 +6681,13 @@
         <v>1004</v>
       </c>
       <c r="B306" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F306" s="0" t="s">
         <v>303</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F306" s="0" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -6704,33 +6725,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -6739,18 +6760,18 @@
         <v>1000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
@@ -6759,18 +6780,18 @@
         <v>500</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2</v>
@@ -6779,19 +6800,19 @@
         <v>500</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>3</v>
@@ -6800,19 +6821,19 @@
         <v>200</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>4</v>
@@ -6821,19 +6842,19 @@
         <v>200</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>5</v>
@@ -6842,19 +6863,19 @@
         <v>200</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="G7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>6</v>
@@ -6863,19 +6884,19 @@
         <v>200</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="G8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>7</v>
@@ -6884,18 +6905,18 @@
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>8</v>
@@ -6904,18 +6925,18 @@
         <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C11" s="22" t="n">
         <v>9</v>
@@ -6924,19 +6945,19 @@
         <v>200</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="G11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C12" s="22" t="n">
         <v>10</v>
@@ -6945,19 +6966,19 @@
         <v>200</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="G12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11</v>
@@ -6966,27 +6987,27 @@
         <v>10000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6998,10 +7019,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>13</v>
@@ -7010,10 +7031,10 @@
         <v>10000</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -7035,7 +7056,7 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7050,252 +7071,252 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="28"/>
       <c r="B2" s="28" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C2" s="28" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28"/>
       <c r="B3" s="28" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C3" s="28" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="E3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C4" s="28" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C5" s="28" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="E5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C6" s="28" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="E6" s="28"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="28"/>
       <c r="B7" s="29" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C7" s="28" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="28"/>
       <c r="B8" s="29" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C8" s="28" t="n">
         <v>7</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C9" s="28" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E9" s="28"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C10" s="28" t="n">
         <v>9</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C11" s="28" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E11" s="28"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="28"/>
       <c r="B12" s="29" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C12" s="28" t="n">
         <v>11</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="28"/>
       <c r="B13" s="29" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>12</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C14" s="28" t="n">
         <v>13</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="28"/>
       <c r="B15" s="28" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C15" s="28" t="n">
         <v>14</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="28"/>
       <c r="B16" s="28" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C16" s="28" t="n">
         <v>15</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
       <c r="B17" s="28" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C17" s="28" t="n">
         <v>16</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E17" s="28"/>
     </row>
@@ -7305,336 +7326,336 @@
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="33"/>
       <c r="C21" s="20" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="34"/>
       <c r="C22" s="20" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="35"/>
       <c r="C23" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="36"/>
       <c r="C24" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="37"/>
       <c r="C25" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="38"/>
       <c r="C26" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="28"/>
       <c r="B30" s="28" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C30" s="28" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E30" s="28"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="28"/>
       <c r="B31" s="28" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C31" s="28" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="E31" s="28"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C32" s="28" t="n">
         <v>3</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C33" s="28" t="n">
         <v>4</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E33" s="28"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C34" s="28" t="n">
         <v>5</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E34" s="28"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C35" s="28" t="n">
         <v>6</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C36" s="28" t="n">
         <v>7</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E36" s="28"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="28"/>
       <c r="B37" s="29" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C37" s="28" t="n">
         <v>8</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="E37" s="28"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C38" s="28" t="n">
         <v>9</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E38" s="28"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C39" s="28" t="n">
         <v>10</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="28"/>
       <c r="B40" s="29" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C40" s="28" t="n">
         <v>11</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="28"/>
       <c r="B41" s="29" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C41" s="28" t="n">
         <v>12</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="28"/>
       <c r="B42" s="29" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C42" s="28" t="n">
         <v>13</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="28"/>
       <c r="B43" s="28" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C43" s="28" t="n">
         <v>14</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C44" s="28" t="n">
         <v>15</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="28"/>
       <c r="B45" s="41" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C45" s="28" t="n">
         <v>16</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="28"/>
       <c r="B46" s="41" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C46" s="28" t="n">
         <v>17</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="E46" s="28"/>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="28"/>
       <c r="B47" s="41" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C47" s="28" t="n">
         <v>18</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="E47" s="28"/>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="28"/>
       <c r="B48" s="28" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C48" s="28" t="n">
         <v>19</v>
       </c>
       <c r="D48" s="41" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="E48" s="28"/>
     </row>
@@ -7643,21 +7664,21 @@
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>4</v>
@@ -7672,7 +7693,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>1</v>
@@ -7685,12 +7706,12 @@
         <v>2</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>1</v>
@@ -7705,7 +7726,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>4</v>
@@ -67043,7 +67064,7 @@
   </sheetPr>
   <dimension ref="B1:Z35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -67180,7 +67201,7 @@
         <v>1</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67223,7 +67244,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67266,7 +67287,7 @@
         <v>1</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67319,7 +67340,7 @@
         <v>1</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67372,7 +67393,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67425,7 +67446,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67478,7 +67499,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67531,10 +67552,10 @@
         <v>0</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="W13" s="1" t="n">
         <v>1</v>
@@ -67599,10 +67620,10 @@
         <v>0</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="W14" s="1" t="n">
         <v>1</v>
@@ -67667,10 +67688,10 @@
         <v>0</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="W15" s="1" t="n">
         <v>1</v>
@@ -67735,10 +67756,10 @@
         <v>0</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="W16" s="1" t="n">
         <v>1</v>
@@ -67803,10 +67824,10 @@
         <v>0</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="W17" s="1" t="n">
         <v>1</v>
@@ -67871,7 +67892,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68209,900 +68230,900 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="77" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="G1" s="78"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="0" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="0" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="0" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="0" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="0" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="0" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="0" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="0" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="0" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="0" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="0" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="0" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="H175" s="0" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="H176" s="0" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="0" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="0" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="79" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="79" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="79" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="79" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="79" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="79" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="79" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="79" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="79" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="79" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D207" s="0" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="E207" s="0" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="F207" s="0" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="G207" s="0" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="I207" s="0" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D208" s="0" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="E208" s="0" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="F208" s="0" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="G208" s="0" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="H208" s="0" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="I208" s="0" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C209" s="0" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -69173,7 +69194,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C216" s="0" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D216" s="80" t="n">
         <v>1300</v>

</xml_diff>